<commit_message>
Get daily reddit data: Tue Mar 11 08:11:36 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_16.xlsx
+++ b/data/collected_data/2025_03_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C503"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3440 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1j8lo2k</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Hole in nail after press ons</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ceqbskkho0oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1j8kue9</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>More Spring Vibes</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/du2ww0k6d0oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1j8kq5k</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Searching for long lasting nail polishes</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8kq5k/searching_for_long_lasting_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1j8k0j0</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Latest DIY set featuring cinnamoroll</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8k0j0</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1j8jv8f</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Before it became vampire nails:</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kmob0jjg00oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1j8jnxg</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>I'm new here ✨</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8jnxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1j8jnli</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Opinions please, which is better?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8jnli</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1j8jfpq</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Shein press-ons... pleasantly surprised</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aaao0h5avzne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1j8ivk9</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>First time trying out gel nail polish!</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkekedu0pzne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1j8ho75</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Most sparkliest Gel Nails I've done on myself</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8ho75</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1j8he4s</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swd7xvcq9zne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1j8gwae</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Spring inspired custom press-ons 💗💗💗</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8gwae</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1j8gvrn</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Why don’t you explain it to me like I am 5 (years old).</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8gvrn/why_dont_you_explain_it_to_me_like_i_am_5_years/</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1j8gmav</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Painting a maleficent nail set on myself 🫶🏼 I'm so mad it looks so similar irl but not on camera! 🥲🤣 Portrait done - now the rest of the nails 💅</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lbh799m2zne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1j8fefy</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>DIY french tips</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8fefy</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1j8fy2d</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Can I Do Gel Nails Without Extensions or Fake Tips?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8fy2d/can_i_do_gel_nails_without_extensions_or_fake_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1j8fvjf</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Some nails I have done</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8fvjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1j8fn9o</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Fossils (contains real bits of fossils) 🦖🦕</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8fn9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1j8ffc5</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Unsure how I’m feeling about these St. Paddy’s Day nails</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfc12jy0syne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1j8fctm</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Toy Story nails i did on myself</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8fctm</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1j8f9je</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>My nail tech is awesome!</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3ezbk8mqyne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1j8evea</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Would you believe this polish came from the Dollar Tree?? 😍</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8evea</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1j8eoco</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>i ♡ a good animal print 🦓</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8eoco</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1j8e5zb</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>How to rock neutrals?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8e5zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1j8e4e5</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Home nail tech questions</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8e4e5/home_nail_tech_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1j8e0r5</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>What do you think about these before and after?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8e0r5</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1j8d2o2</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Just got press ons - HELP!</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8d2o2/just_got_press_ons_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1j8d96e</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>My GF made me hybrids and I stopped biting!</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzwill6e9yne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1j8dhjp</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Too early for Easter nails, so went for a classic French Tip!</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1p7te1bbyne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1j8dh1n</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>are the nail art brushes from Kiara Sky any good?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8dh1n/are_the_nail_art_brushes_from_kiara_sky_any_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1j8d6qj</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>I work as a barista - any tips on how to make sure falsies don't come off?</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8d6qj/i_work_as_a_barista_any_tips_on_how_to_make_sure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1j8d2ts</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>New nails. My girl did so good 😍🥰</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6lxf36x7yne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1j8cq9q</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Busco chicas que quieran aprender todo sobre la manicuria !</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8cq9q/busco_chicas_que_quieran_aprender_todo_sobre_la/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1j8cp2f</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Daisy the pig by sinful colors</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nskcqtr4yne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1j8cmmw</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Not done but Ive been on a girly kick lately</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8cmmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1j8cbv8</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>My unprofessional tutorial on the vampy cat eye trend</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/61qh9va31yne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1j8bsth</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>JELLOJELLO Peel Off Base &amp; One Kill Remover - First Impressions</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8bsth</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1j8c9c3</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>My nails after acrylics</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8c9c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1j8avxq</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Sonny Angel Nails✨</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycavsd53rxne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1j8baij</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Back in my chrome nails era 🤍🌸🌸</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tp4ozs14uxne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1j8avkl</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>St. Patty’s ready</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10uvfja0rxne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1j8akzq</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Only the second set of acrylics I've ever done, on myself. Mourning my cuticles tho 😭</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wbg5nnkhoxne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1j8aiur</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>My attempt at porcelain nail art?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8aiur</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1j8ahi6</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Obsessed with magnetic nail polish 🤩</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gy22cpi0oxne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1j8ad4l</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Magnetic peach nails 🍑</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/trm1vzl1nxne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1j89z20</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Favorite Clean-Up Brush?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j89z20/favorite_cleanup_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1j89tr8</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>What do my almond nails look like? They are simple but I loved them</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a76kv513jxne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1j89lkz</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Did my husband’s nails last night 🥰</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3wju7dghxne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1j892bx</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Rubber base at home</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j892bx/rubber_base_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1j88sc2</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>FRESH NEW SET ON THE HOUSEEE</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j88sc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1j85efx</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Sanrio press ons💕✨💅🏼</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aboeue0fmwne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1j882za</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Polka Dots</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j882za</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1j87rfo</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Mystery Manicure is giving coronation Arwen ✨💚</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j87rfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1j87qfl</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Dip powder</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j87qfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1j87c5i</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Saint Patrick’s Days nails bc I don’t want to get pinched lol</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/igd4j25k0xne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1j8721e</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Showing my cat my fresh nails</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8721e</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1j86rle</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Any advice on how to quit biting nails?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j86rle</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1j86r8o</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Got my horrible manicure fixed</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5urpsey3wwne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1j86o68</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>These are my natural nails</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hcsil8hvwne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1j86ckc</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>March’s color - OPI “Love You So Munchkin”</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljpl7186twne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1j867ws</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Press ons of the week 🍵🪷</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j867ws</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1j8673r</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>First time doing chrome powder at home. Any advice where to buy more?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aq1y4is2swne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1j866i8</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>I’m improving:D</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j866i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1j86300</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Kiss French Tip Nails!!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zdnugn58rwne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1j85y4v</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/377u62l9qwne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1j84h28</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>What kind of glue should I get?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c7pc67lfwne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1j8536m</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Made a fruit series</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8536m</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1j84nu0</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Disco ball nails 🪩</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j84nu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1j84a8h</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Tortoiseshell, yay!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j84a8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1j842lb</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>My natural nails because my ADHD doesn’t let me stop biting my cuticles….</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3uaca3lmcwne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1j83f2u</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>lucky charms inspired 🌈🩷🍀</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j83f2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1j83hd4</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Rave nails for a friend - obsessed with how these turned out!</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9xrq2bc8wne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1j839om</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Back to natural nails 🤗</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jiluu0vq6wne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1j834z1</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>The color red is a trend</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4udktlr5wne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1j822mk</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Decorated Broke Nail</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gewpoxb1yvne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1j82s1c</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Lace foil nails!</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j82s1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1j830cz</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Question About Fill Ins!</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j830cz/question_about_fill_ins/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1j82wuf</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Two sets from the same order! What do you think?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j82wuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1j82qmj</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>So Obsessed 🥰</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9kb39vv2wne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1j82msm</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>How do these look?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vx969g442wne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1j82k9j</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Spring cleaning</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j82k9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1j82guy</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Stained glass on mostly natural nails</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j82guy</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1j8214f</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>silver chrome and black is always fun</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8214f</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1j81j0y</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I am start the day with a grey shade</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n52pcn9ztvne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1j7xyn6</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>should i swap? and if i do, which one?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j7xyn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1j7z126</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Accent nail help? (Inspo Credit alynails.salonandacademy on insta)</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8esosl9avne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1j8172e</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>I can't get my semi-permanent nail polish more than a week</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8172e/i_cant_get_my_semipermanent_nail_polish_more_than/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1j8100h</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Green for St Patrick’s day!</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxn051rypvne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1j80vrm</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Spring is here! 🌸</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jsnkzi72pvne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1j80mmj</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>need advice with basic things</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3v9ztav1nvne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1j80kgo</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Been awhile</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j80kgo/been_awhile/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1j80j0k</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Desperately need help</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j80j0k/desperately_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1j80gg2</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>My current set 🥺🤍</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xe1igwlplvne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1j80des</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Thoughts on this??</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j80des</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1j80d2a</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Short, simple</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j80d2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1j806g9</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Gel polish keeps lifting</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6vyq2kkjvne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1j7zys3</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z70qe4gshvne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1j7zsv2</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>$60 😍 I love them. Second time getting my nails done after an awful experience my first time.</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j7zsv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1j7zsnn</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Best nail tech in Newfoundland</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szxembeggvne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1j7zmrn</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Flakie shorties</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i2rjtpl5fvne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1j8k70w</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Sudden Chill 👻</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8k70w</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1j8k1fi</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Color Club - Angel Kiss</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8k1fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1j8jyk9</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>shipping Korean gel nail products to the US? is it possible/worth it to try?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j8jyk9/shipping_korean_gel_nail_products_to_the_us_is_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1j8jefl</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>No horseshoe magnet, no problem (magnet setup included)</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8jefl</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1j8jb7t</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>teh cozy babby mani</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4m01l9cqtzne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1j8iq0q</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Are my nails too damaged for acrylics?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8iq0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1j8io8u</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>St. Patrick’s Day🍀</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8io8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1j8im6h</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Indies, where have you been all my life?</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qq8zxzc5mzne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1j8iiu9</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Separated glitter?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4yeko96lzne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1j8iaj2</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Thermals are fun!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cbjexbrizne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1j8hpay</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>For the love of velvet</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sfgpw67uczne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1j8hi3u</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>indie brands from etsy, part 3: Happy Rudy</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8hi3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1j8hgzk</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Polishes like Mooncat’s The Stolen Kiss?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3x0mfzjazne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1j8h5gy</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Anybody else match polish to their hair?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8h5gy</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1j8h1s9</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>recent manis + pup tax</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8h1s9</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1j8gkoq</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Did my mom’s nails for her belated B-day</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8gkoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1j8gdd7</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Performance Blue nail polish</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvktjf0e0zne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1j8fnsn</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Fossils (contains real bits of fossils) 🦖🦕</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8fnsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1j8fk72</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Mooncat Stumped. Batch issue or was I expecting something it's not?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8fk72</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1j8etvh</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Thoughts on my nail tech</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4453h</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1j8esxl</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Dazzle Dry - Pink Plume</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8esxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1j8er5s</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>received my first-ever polish pickup order last week! immediately committed to another order for march lol</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8er5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1j8ell9</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Glitter Grabber thickening</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/we6acrptkyne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1j8ei98</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>I can’t do gels because I get bored after 3 days 😂</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8ei98</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1j8e2vc</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>First tricolour skittle of Autumn 🍂</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8e2vc</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1j8dvai</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Need a dupe for this sort of magenta/neon purple pink shade!! As eye-searing as possible!</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8dvai</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1j8cj5q</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>first sunny day in awhile</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8cj5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1j8brrk</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Desperado Under The Stars (with extra stars)</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bbswevwrxxne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1j8bmbi</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Looking for flowers/florals....</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j8bmbi/looking_for_flowersflorals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1j8at8g</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>This Weeks Manicure</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1o9gmdiqxne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1j8as1t</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Getting back into magnetics</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iou089h7qxne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1j8as91</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Are we still doing “soap” nails? 🫧</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/petkhikaqxne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1j8aly6</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Why did this happen?</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3o3pp9wxoxne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1j8am14</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Part 2 of my first lurid lacquer order!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8am14</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1j8aiul</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>First Lurid Lacquer order!😍</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8aiul</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1j8a1bi</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Kicking myself for not checking the label, please assist!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8a1bi</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1j89zvl</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Finally got my first magnetic!!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j89zvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1j89vql</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>I am a beginner to nail care, how do I make my nails healthier?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j89vql</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1j89rrz</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>What is your favorite purple polish?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j89rrz/what_is_your_favorite_purple_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1j89iyv</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>arcana lacquer - the magician ✨</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ehxeuidwgxne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1j898wj</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Searching for a polish the formula of Mooncat Dragon Scales but in the color of Holo Taco Fallen Flake</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j898wj/searching_for_a_polish_the_formula_of_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1j897z4</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>gentlemen, throw me your sluttiest, coral-iest, summer-iest, violent hot pink/coral/orange</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j897z4/gentlemen_throw_me_your_sluttiest_coraliest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1j88rg1</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Do you feel for me the way I feel for you?</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57sqt5nbbxne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1j8865l</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Swatch Comparison Request: Holo Taco Amber Apathy vs ILNP Legacy</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j8865l/swatch_comparison_request_holo_taco_amber_apathy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1j87nbt</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>What tha shift?!?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j87nbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1j87k0m</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Nosferatu by BKL 🦇🩸</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j87k0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1j87jgy</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>small LynB haul!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4yv7xj52xne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1j873pg</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>After weeks of searching, I think I found the perfect polish to match Mantis' nails!</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j86zmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1j85x85</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Venting about this bottle</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/en9pqmtypwne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1j85bac</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Can I still get a manicure with my broken nail?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j85bac</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1j8568y</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Batsquatch in the wild</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8568y</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1j853yg</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>❗️TW for gross pic on second slide❗️After 4 months of no polish, I put on my first mani today!</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j853yg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1j84jv9</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Achievement Unlocked: Painted a pet hair on to my nail. Luckily it's a thermal polish and you can only see it when my hands are warm, which is never.</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j84jv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1j84aow</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Lurid prototypes!!</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j84aow</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1j83ron</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>dupes for alchemy lacquers oddities?? 😭</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1fa0wjfawne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1j839vi</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Still in love with this polish</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j839vi</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1j82zbj</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Cracks/chipping</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j82zbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1j82z6s</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>horseshoe magnet…</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j82z6s/horseshoe_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1j82q4e</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Rainbow for spring🌸💜🌈</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j82q4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1j82q0p</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>nail polish empties 😮</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njrygvq6tepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1j82ppb</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>The comparison nobody asked for, Patina Lite vs Serpents of Eden</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8hlb6vmh2wne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1j82kpf</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>This looked cuter in my head</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mimw30p1wne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1j81yka</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Help me find a bright red/orange nail polish that isn't a gel?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j81yka/help_me_find_a_bright_redorange_nail_polish_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1j81y1z</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Does anyone on here use the Nail Boo gel or dip powder products? If so, why or why not?</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j81y1z/does_anyone_on_here_use_the_nail_boo_gel_or_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1j81uhv</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>My first Vanessa Molina 🥰</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j81uhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1j81sfe</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>My little dopamine boost via Lurid Lacquers Indomitable</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ubr9f0hzvvne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1j81f0f</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>The Lovely Flowers by Bees Knees Lacquer 🦇🩶</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j81f0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1j819qm</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Just casually sitting on my kitchen floor admiring my nail polish because the lighting is fantastic down here</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4q183dgvrvne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1j818nh</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Love it when drugstore delivers! 💅</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j818nh</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1j815bx</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Nail Polish Color Hit Full Moon Party</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>/r/Sephora/comments/1j80xd3/nail_polish_color_hit_full_moon_party/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1j80to1</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Does Daybreak work on me?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j80to1</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1j80etw</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Mani of the week</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4v9u6loclvne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1j7zzky</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>impossible to capture in photos 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j7zzky</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1j7zmt2</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquer can have every last cent to my name.</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j7zmt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1j7zi1r</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>I can no longer resign to a crème or just a solid manicure 💅</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9rgvedn3evne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1j7zdhv</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>norpsilocin in the sun 🤩</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p8hhodxscvne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1j7z9si</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Hypoallergenic Gel Nail Strips?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j7z9si/hypoallergenic_gel_nail_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1j7yzkf</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>my first gel polish at homs</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j7yzkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1j7yq2q</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Got complimented by two little girls at the playground.</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2j0i1i6l7vne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1j7ypoh</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>First time wearing this since I got it almost a year ago. I’m a fan!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j7ypoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1j7yd9f</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Enjoying the shifty deliciousness of Psilocybin</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/txysvsag4vne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1j7ybh3</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>I need a polish dupe for these gel nail wraps. Any suggestions?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/oFPNXC8.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1j7xgne</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Balou and Enemies to Lovers</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j7xgne</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1j7x8az</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Please help! Broken thumb nail 😢</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j7x8az/please_help_broken_thumb_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1j7v6p3</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j7v6p3/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1j7v6oc</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j7v6oc/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1j7v6ns</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Second Clionadh haul</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02v3r4fq5une1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1j7trkb</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>how do you like to organize/display your swatch sticks?</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j7trkb/how_do_you_like_to_organizedisplay_your_swatch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1j7trdc</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Satisfied with my skittle</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6475z4i2mtne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1j8gsv1</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>3d nail sculpt</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j8gsv1/3d_nail_sculpt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1j8gmj4</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Painting a maleficent nail set on myself 🫶🏼 I'm so mad it looks so similar irl but not on camera! 🥲🤣 Portrait done - now the rest of the nails 💅</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inrsjs6o2zne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1j8g86j</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>First try, done with non dominant hand</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgi46gu3zyne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1j8g746</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>art dump</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8g746</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1j8fhty</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>What is this base color???</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ac83ywzmsyne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1j8dq9s</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Hard gel</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nivj35nbdyne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1j8c08r</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Second ever attempt at nail art! Doing my best, thoughts?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0ysl9yizxne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1j8a3pb</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Needed some quick nails for a uni presentation: now I have the power of weird alien nails and anime on my side, wish me luck 🤪</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8a3pb</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1j895ch</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Gothic set 💀</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/je4cy3o4exne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1j886nm</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Cybersigilism Barbie vibes</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j886nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1j84w4q</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Jujutsu Kaisen or One Piece 🏴‍☠️</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j84w4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1j84i6f</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>March 2025</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zt89rhusfwne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1j7uhkf</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Water nails for summer? 🌊💅</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kkcr8s9dwtne1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Mar 12 08:11:31 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_16.xlsx
+++ b/data/collected_data/2025_03_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C503"/>
+  <dimension ref="A1:C688"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8984,6 +8984,3151 @@
         </is>
       </c>
     </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1j9e8vw</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>I sure as hell wanted long nails 🩷</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/770oawtpl7oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1j9dokv</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Hello 🌈 I'm new here</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0z2fhihgg7oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1j9dnlm</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Cat eye for bestie n me!</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9dnlm</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1j9cyih</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>nailene ultra quick vs Infilila?</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9cyih/nailene_ultra_quick_vs_infilila/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1j9cd4k</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Spring Time Flair</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3h46ka1947oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1j9boa9</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Golden springtime✨🌼</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usfeq8b3y6oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1j9bkzv</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Barbie pink holo nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a5qk37kcx6oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1j9b1as</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Not my best, but I'm obsessed with the color</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnvdd8ges6oe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1j9aplr</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>I've been doing my nails myself for about 6 months! It's so therapeutic!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c4ffunbwo6oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1j96dyk</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Nail shape</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9eqjsc75m5oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1j98dwx</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Need advice please 🙏🏻😫</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j98dwx/need_advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1j99gb5</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Looking for a solution</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j99gb5/looking_for_a_solution/</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1j9a90t</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Found this nail salon in Austin on TikTok and never looking back. What do we think?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iljmmwd8k6oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1j99t4i</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Some butterflies for spring!</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j99t4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1j99qut</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Hypnotized by this cat eye.  😍</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j99qut</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1j99blg</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Press ons I made ☘️</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j99blg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1j98wgu</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Which shape looks best? Need confirmation before video</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j98wgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1j98sjm</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>My nails and my tattoos 🛐🛐🛐</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s18kmj7g66oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1j98n38</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Is 2 weeks long enough to get a refill? There’s enough natural nail showing that it’s made a noticeable gap. I’m also tired of the French tips/design I got lol</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j98n38/is_2_weeks_long_enough_to_get_a_refill_theres/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1j98jqf</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Self made🤍</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oej035o946oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1j98ixv</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Do you like it?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s69nfmn346oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1j98gpw</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Nails I did yesterday. Rate my work.</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j98gpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1j97o4g</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Amber Cat Eye Press Ons</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onaonc7nw5oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1j97rrk</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>I’ll forever be obsessed with neutrals 🥰</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j97rrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1j97lad</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Enjoying my fresh pop of pink!</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1rptk3v0w5oe1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1j96gri</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Any treatment to make them grow?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j96gri</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1j96bca</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>new press ons 🫐</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ak7n7ntil5oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1j95p68</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>🍏</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j95p68</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1j92rcw</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Does anyone know what the difference is between these two files?</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkuxlxift4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1j94v2w</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>My friend told me these look like panties and I can’t unsee it 😭</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhxa5ion95oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1j95ie7</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Question about nail allergy</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j95ie7/question_about_nail_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1j95azd</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>my new favorite mani ever</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j95azd</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1j9594j</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>first draft of a set I plan on selling, what do you think i should call it?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9594j</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1j954dx</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Tweed Nails 🩵</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j954dx</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1j953xu</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Press-on nails. What do you do if there are not enough sizes in a set to fit all you nails?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j953xu/presson_nails_what_do_you_do_if_there_are_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1j94p1c</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Cute little nails uwu</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r55dnlrh85oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1j94nck</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Lisa Frank bringing in spring 🐯🩷💜💙✨</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j94nck</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1j94jbu</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9y1xl1975oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1j949gb</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Milky White Russian manicure 🤍</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j949gb</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1j9471n</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Looking to buy from someone Cuticula Hummingbird Glass</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3id6ggl45oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1j93kdx</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>They look a bit boring but I really like my nails.</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eun6wbemz4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1j93jw3</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>St. Patrick’s Day</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsm5c8biz4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1j93fsv</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Electric Nail File Recommendations</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6t6uf2my4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1j939z8</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>All the sets I’ve gotten till now (24f)</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j939z8</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1j93682</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Flat nail beds?</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j93682</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1j9357f</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>The gel bottle keeps bubbling under light?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9357f</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1j92e2j</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>chrome hearts inspired set</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j92e2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1j91kno</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>can gel press ons cause allergy?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j91kno/can_gel_press_ons_cause_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1j92bua</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Happy Spring!</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j92bua</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1j926qx</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Birthday month/St.Paddy's Day nails</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j926qx</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1j9233h</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>a bit messy but i’m happy with them</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljmzy63co4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1j922a7</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Primer and Gel: same brand?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j922a7/primer_and_gel_same_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1j920me</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Birthday Nails! 💕</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3fgwthsn4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1j91j3e</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Spring flowers 💐</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqswegt7k4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1j919k3</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Spring mushie set, I love creating fun nails!</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z72588zai4oe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1j913x1</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>🐝✨</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j913x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1j90ujt</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>I found Glamnetic nails at Canadian Winners.</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0vgynd7f4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1j8tnxm</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>What are we doing with our nails??</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8tnxm/what_are_we_doing_with_our_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1j8r1ow</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Giving up gel and my nails look weird</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rsos8i1e2oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1j90h4y</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>simple but effective! ✨</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eo3cmlhec4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1j90gq9</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Some fresh birthday nails! 🥳</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yajeqttcc4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1j8zh4b</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Going from regular polish to Gel</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8zh4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1j908y9</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Saint Patrick's Day mani on natural nails!</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hcnq9opma4oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1j8zkv2</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Decided to change something</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8zkv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1j8zjuc</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>My Lucky Charms set for St. Paddy’s Day! So obsessed with how these turned out!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8zjuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1j8zcbx</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Is this a coloured chrome? Or coloured nails with pearl chrome? Nails done by Gold Digger</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6b5r93744oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1j8zbe1</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>color change cuties 💖☺️</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jh3yn29044oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1j8zavu</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>My Lucky Charms nails for St. Paddy’s Day! 🌈 🍀 ⭐️</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8zavu</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1j8r5kr</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>help!</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6yk91ixe2oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1j8so6n</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Help me!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8so6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1j8yy07</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>What kind of mani is this?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gje8vqza14oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1j8y89z</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>What do you do after getting a bad manicure?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8y89z/what_do_you_do_after_getting_a_bad_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1j8l4ax</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Builder gel to protect nails from Press-On damage?</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8l4ax/builder_gel_to_protect_nails_from_presson_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1j8q0rr</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>What nail design should i choose?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8q0rr</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1j8rwxk</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>i honestly can't decide if i like them</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8rwxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1j8y75l</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>My nails grew out and were getting too long so I fixed them up a bit. What do y’all think? (before and after)</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8y75l</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1j8lwbh</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>How can i keep all my nails one length?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8lwbh/how_can_i_keep_all_my_nails_one_length/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1j8ttsf</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Cock a doodle Doom</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8ttsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1j8ux3r</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Builder Gel Fill Hurting?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8ux3r/builder_gel_fill_hurting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1j8x6mp</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>rubber base nail polish?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8x6mp/rubber_base_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1j8wqjw</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Tried a “design” for the first time!</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knfxj3u8l3oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1j8wxmx</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Lifting with Bio Seaweed Gel</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8wxmx/lifting_with_bio_seaweed_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1j8wvwh</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Has anyone tried gold leaf on their nails?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8wvwh/has_anyone_tried_gold_leaf_on_their_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1j8wrvq</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Ready for spring! 🍀 🌷 🪻 🌼 💧</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8wrvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1j8wqte</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Wanted to be festive for St patty’s day. Are they as bad as I think?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/majsphval3oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1j8wkac</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Kiss X Tend</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nc8befzj3oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1j8whhe</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>For those who do their own nails: do you ever get them done too?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8whhe/for_those_who_do_their_own_nails_do_you_ever_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1j8weti</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>A polish I've gone back to a million times over the last decade +</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8weti</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1j8wcl7</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Tried doing gel myself for the first time</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8wcl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1j8vwb4</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Need recommendations</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j8vwb4/need_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1j8vis3</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Did my nails!!</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdsn7effc3oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1j8viok</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Wanted to show off my nails my tech did a fantastic work</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2sff9wgfc3oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1j8v1ib</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>This was a nightmare to do, any advice for doing French pedicures? My white lines felt shaky af but I think we got there in the end</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7dvfskx83oe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1j8v1fq</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>French…with a twist</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myyb61xw83oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1j8v0cw</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>💙</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8v0cw</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1j8uuxq</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>I'm new to doing my own nails but I love how these GLOW.</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8uuxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1j8usf7</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>so obsessed with my pink chrome nails ! 🎀</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tad833g273oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1j8ujbh</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>My newest addiction</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvta8us853oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1j8u4eg</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>just got this design!! what do you think??</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kh40x15723oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1j8u3x6</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>teal for spring</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8u3x6</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1j9dvmu</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>just got my cracked polish order 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc5r0uvai7oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1j9b98l</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Lethal Cosmetics Dexter Review/Swatches</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9b98l/lethal_cosmetics_dexter_reviewswatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1j9b8fz</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>The face behind the brand</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9b8fz/the_face_behind_the_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1j9a6ig</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>From the Cottagecore Collection at Holo Taco</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qylerx3jj6oe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1j99re2</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Help! My nails look awful after using gel.</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j99re2</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1j99ko1</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Request</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lq76jurmd6oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1j99iyi</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>First thermal!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j99iyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1j99ak7</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Flower Child makes everything better! (Last Batsquatch post, I promise)</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gx7245xya6oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1j98kcu</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Diseño ideal para una novia . Que dicen ??</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1g8znu4a46oe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1j98aw5</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Cracked nail files a disappointment...?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j98aw5/cracked_nail_files_a_disappointment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1j9817x</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Jennifer Lawrence’s nail polish in American Hustle. Help me find this color!  Took place in 1978, it’s a reddish color.</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4jwj1tqz5oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1j97c93</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Clionadh x2</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j97c93</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1j964wm</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Those of you who switched from keeping polish in Helmers to something else, what other drawer organizer units do you recommend? Any to avoid?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j964wm/those_of_you_who_switched_from_keeping_polish_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1j95zcd</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>anyone else have a “white whale” polish?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4v2ydbsi5oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1j95p8o</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>A blue polish to fit in this collection?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44z3431gg5oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1j955y8</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Subtle yet sparkly!</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3f40lxl5c5oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1j94ywa</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Maybe she’s born with it… maybe they’re repainted press ons 😄</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j94ywa</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1j93vlo</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Hear me out</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t47y4m6w15oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1j93q7u</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>In love with smeet frog 🐸</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qimw2b5v05oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1j93nzx</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Shoutout to Cracked Polish</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j93nzx/shoutout_to_cracked_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1j92g3x</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>More Batsquatch! Ft. The Silent and Flower Child</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j92g3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1j92923</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Happy Spring !</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j92923</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1j923ae</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Birthday month/St.Paddy's Day nails</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j923ae</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1j91kv3</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Rose Quartz Marble</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wty03vdkk4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1j91iiz</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>The annual nail polish reorg - Switching back to color from 'flavor'</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k3ekgw3k4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1j91eq3</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>looking for a stamping polish rec</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j91eq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1j91dgn</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Layering</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kv9lxf04j4oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1j90xf7</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>decided to try seafoam green for Saint Patrick’s!</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p6hyxttrf4oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1j90n4k</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Was a nail biter for 26 years and tried everything- so proud I stopped!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j90n4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1j9087u</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Manifesting spring weather with Essie Bling It!</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iem0ouqka4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1j8zztl</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>fairy dust in the afternoon ✨</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8zztl</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1j8zkat</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Come on Barbie, let’s go Barbie!</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8zkat</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1j8zgbd</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Swirls and Flowers</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8zgbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1j8yyif</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Broken nail advice needed</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr1cbioe14oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1j8yiuw</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>My first Lurid haul, inc. prototypes!</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8yiuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1j8xuu9</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Wide nail beds</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j8xuu9/wide_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1j8xsmd</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>HELP! Need suggestions for doing wedding nails for a friend</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ztwmaius3oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1j8xro5</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Synth abstract valentines from last month</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vp2cwqps3oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1j8wu7u</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Regular nail polish after 4 weeks</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8wu7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1j8wpfv</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Help? Bought RCM to do at home.</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8wpfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1j8wjfa</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Death Valley Nails Polish Thinner Recs?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j8wjfa/death_valley_nails_polish_thinner_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1j8wh7v</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>I should have bought this sooner 😭</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k7zdohhcj3oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1j8vzlh</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Tried color matching - anyone have other ideas?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehkuk4zsf3oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1j8vwbe</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Looking for this but in raspberry?</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14qaar13f3oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1j8uxc6</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Just a Trans Woman Excited to Show off my St. Patrick's Day Nails</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8uxc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1j8unf7</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Prugly?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8unf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1j8uja3</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Sparkly in every light!</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8uja3</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1j8ugd6</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>So excited for spring nails</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8ugd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1j8tud4</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Cock a doodle Doom</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8tud4</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1j8t2j9</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Clionadh has the best magnetics hands down</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jlrb1f69u2oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1j8syx2</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Witchful Thinking</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mnizdugt2oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1j8s88z</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Has anyone tried the Abomination Cosmetics Frost toppers?</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8s88z</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1j8s77d</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>My absolute favorite nail polish!(excuse warped nails from psoriasis)</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8s77d</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1j8r46y</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Favorite greens and blue/greens?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j8r46y/favorite_greens_and_bluegreens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1j8qoc9</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Swirly blue opal-y vibes</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8qoc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1j8qjwm</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Back in the game</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e70d7aju92oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1j8qesk</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>🖤💚Memphis Suit🩷🤍</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8qesk</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1j8g75d</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Did my first three color gradient</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m29pl3guyyne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1j8jwjv</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>shipping Korean gel nail polishes to the US? possible?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j8jwjv/shipping_korean_gel_nail_polishes_to_the_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1j8o5f5</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Green Goddess 🧚🏻</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8o5f5</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1j8o486</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>ILNP</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7juvao77l1oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1j8n8li</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Happy with this combo of Mc, Monarch and cdc</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8n8li</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1j8mrse</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Building My Dream Nail Polish Collection—What Are Your Go-To Shades?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j8mrse/building_my_dream_nail_polish_collectionwhat_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1j9dab0</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>St. Patrick's Day Nails</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cx8jylgoc7oe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1j99q94</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>First time with chrome!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j99q94</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1j97hx0</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Teaching myself dip nails.</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lesnch0av5oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1j96x5i</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Need tips on Brushes</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j96x5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1j96pwa</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Stamping plate help</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j96pwa/stamping_plate_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1j957vm</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>first draft of a set I plan on selling ! :) what should i call it?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j957vm</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1j92w6e</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>New nails,cat eye and chrome💕</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8bwp3kaeu4oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1j92j2f</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>chrome hearts inspired set</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j92j2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1j91tef</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>🐥💐☀️</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3bzk55cm4oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1j911of</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Bling bling nails on my friend</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j911of</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1j8z783</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>I did some mini lava lamps that also glow in the dark</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8z783</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1j8yplt</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Ombre</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vfmt4elz3oe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1j8wpna</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Design suggestions</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocs8g952l3oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1j8w8cy</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Wanted to share this Ombre I did before doing the nail art</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpw2mbnlh3oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1j8vetr</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>What we think of this one? 🤍</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8vetr</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1j8u9n0</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>my holy [not sponsored, I wish!] grail matte top coat for chrome + pencil/pen/watercolor art! the vendeeni russian matte top.</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8u9n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1j8rlj2</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Is there a difference between the nail police for fake nails vs the real ones?</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j8rlj2/is_there_a_difference_between_the_nail_police_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1j8nypo</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>First time lol</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8nypo</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1j8nujm</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>New set I just made</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j8nujm</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1j82yja</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>First art</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j82yja</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1j7aiz7</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>I love purple 👍🏻</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j7aiz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1j76669</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>need advice with adding charms to nails at home!!</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j76669/need_advice_with_adding_charms_to_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Mar 13 08:11:25 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_16.xlsx
+++ b/data/collected_data/2025_03_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C688"/>
+  <dimension ref="A1:C897"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12129,6 +12129,3559 @@
         </is>
       </c>
     </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1ja6q1t</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Paper towel extensions</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja6q1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1ja6nsg</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Homemade DIY French tips</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja6nsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1ja5ym0</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>💙</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja5ym0</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1ja5dqn</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>I'm literally obsessed with how my nails turned out!</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja5dqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1ja4nly</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>What’s the best shape and length for my hands?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja4nly</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1ja4p3k</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Lavender for spring☀️</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xfriw405eoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1ja4jpz</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Shiny, I love the result</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2et9h8l83eoe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1ja49io</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>My nail tech is a pro!</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2tt46bwzdoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1ja49do</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Need to grow out my nails but I want artificial nails for the meanwhile, what wouldn't be damaging?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ja49do/need_to_grow_out_my_nails_but_i_want_artificial/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1ja3wtz</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Do you like?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bjeh923wdoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1ja3s1s</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Spring nails! 🌼</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol9cyhuoudoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1ja3rhe</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Meyer Lemon China Tea Set</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja3rhe</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1ja3f9t</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>do these sizes seem accurate?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2rrexr1rdoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1ja2wni</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>✨</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja2wni</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1ja1wld</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Did these today!</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffrlcekfcdoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1ja166a</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Chrome French set I did last night</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja166a</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1ja10tl</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Best hard gel brands for the UK without being certified? All I’m finding is IBD on Amazon.</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ja10tl/best_hard_gel_brands_for_the_uk_without_being/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1ja0vvh</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Spring has Sprung 🌺</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0kd2bus73doe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1ja0lve</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Just got my nails done for the first time in almost 3 years!</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja0lve</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1ja08jx</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Does this nail shape fit my hands?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja08jx</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1ja082j</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Please enjoy my green nails 🍀💚</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrizt6fbxcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1ja0799</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Some festive nails I did today 💚</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5nn98ss3xcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1ja02ln</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Help! WARNING GRAPHIC NAIL DAMAGE ON SLIDE TWO</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja02ln</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1ja0301</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>do i have to include glue in my press on sets?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ja0301/do_i_have_to_include_glue_in_my_press_on_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1ja02nw</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Showing off my progress!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja02nw</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1j9znrg</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Advice</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9znrg/advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1j9zlhc</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Tortoise shell &amp; gold press ons</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cz7t91syrcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1j9zj6s</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>🍄</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5dl131grcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1j9zf7b</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Post-Acrylics Nail Rehab Help</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9zf7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1j9z9xh</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Advice on how to help the healing process?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5x5paz9pcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1j9z4ro</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>New set inadvertently matches my latest read 📖🩷</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9z4ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1j9z046</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Started doing nails in September 2024</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46a9jvizmcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1j9ys2w</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Need help with efile drill bits- beginner.</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9ys2w/need_help_with_efile_drill_bits_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1j9ymcr</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Do these nails look odd on me or do I just need to get more used to the style?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9ymcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1j9y7u0</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Love my damaged and dented nails 😓</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9y7u0</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1j9yep5</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Structured clear french tips with irridescent foil</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9yep5</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1j9y77o</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Polygel</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ltgzpbdgcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1j9y61f</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Love these press-ons so much I had to do them on my nails 😍🔥</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cq589l14gcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1j9y523</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>My cat-eye stained glass birthday nails by me 🥳</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9y523</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1j9xgqo</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>fill or full set?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9xgqo/fill_or_full_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1j9xc9g</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Second set of nails done!!</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9xc9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1j9x4av</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>What I asked for vs. What I got - ✨inspo from u/princessn00dle ✨</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9x4av</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1j9wxl3</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>This week’s mani - not sure how I feel</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9wxl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1j9x30n</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Loving my shorties!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/674mhbnl7coe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1j9x0yl</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>I’m not really a good model.</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9x0yl</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1j9wzm1</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>First time trying to do my own nails</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/taowp8mt6coe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1j9wow8</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>🐰Battle Bunny Miss Fortune🔫</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9wow8</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1j9wovh</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Help😭</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9wovh</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1j9whiw</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>These are my natural nails</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hr02gimw2coe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1j9w96g</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>My birthday set! In love</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9w96g</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1j9w1mb</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Manifesting Spring 🌸🌺🌷</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9w1mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1j9v2o0</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Help with my toe nail!</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfy9zbo2sboe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1j9vdk8</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>I love pink</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtogm6l9uboe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1j9uz44</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Bright color for Spring</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9uz44</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1j9utd8</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Is my nail wrecked?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7gww04spboe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1j9uoyk</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>More Birthday month/St.Paddy's Day nails</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7rwtunjdoboe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1j9u1yy</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Tried a new color.</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fk98ykijboe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1j9tl5a</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmlzfro5gboe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1j9trha</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Currently struggling</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9trha</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1j9tcst</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Happy St. Patrick’s Day</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nu06ydwfeboe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1j9ta2p</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Seafoam w chrome 🧜‍♀️ 💚</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9ta2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1j9sxyt</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Is bond needed?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9sxyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1j9s4bm</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Wicked nails</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9s4bm</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1j9se4m</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>To anyone struggling, you can do it!</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9se4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1j9rls8</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Cordless Electric Nail Drill</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9rls8/cordless_electric_nail_drill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1j9rnab</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>I tried Polygel with ombre jelly on top</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7khjt042boe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1j9rds2</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Pearls!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fx9gmzya0boe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1j9rai1</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Super influenced by painterly spring nail art!</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/Dn8hDOI.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1j9r5un</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>My third ever set of nails I’ve done!</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9r5un</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1j9qlgj</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>My first ever set!</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4je444luaoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1j9qjx6</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Pink 🌸 (Depend Polish in Magnolian Courtyard)</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9qjx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1j9qb3t</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Nail Strengtheners</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9qb3t/nail_strengtheners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1j9qbxa</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Can someone give me a beginner’s guide for doing my nails?  I have CND Shellac polish (base, color, and top coat) and a nail light</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9qbxa/can_someone_give_me_a_beginners_guide_for_doing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1j9q71w</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>New design 🌳</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9q71w</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1j9qhdu</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Just made these</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrybccrrtaoe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1j9qezr</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Sunny coffee shop 😍</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9qezr</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1j9p70b</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Struggling to blend gel-x cuticle</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5onhqahkaoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1j9pffi</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Bad shape</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9pffi</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1j9ozrp</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>My press-on nail story (AKA looking for advice on painting, removing, repainting, and reusing press-on nails)</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9ozrp/my_presson_nail_story_aka_looking_for_advice_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1j9oxmm</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Troubles with peeling...</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9oxmm/troubles_with_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1j9gw0s</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Sushi nails for Sushi lunch date</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9gw0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1j9gq4j</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>How to remove charms from regular polish without destroying them?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9gq4j/how_to_remove_charms_from_regular_polish_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1j9l1lg</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Rubber base process lifting</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9l1lg/rubber_base_process_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1j9iaj2</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Biab nails coming off? Beginner</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9iaj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1j9nhr6</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Anyone ordered a bundle from Pamper Nail Gallery before? How long did it take?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9nhr6/anyone_ordered_a_bundle_from_pamper_nail_gallery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1j9nhnv</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Birthday Nails 🍀</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7kkp3y38aoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1j9n3fb</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Que lindas me quedaron :3</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3v3bn975aoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1j9n1gj</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>First time trying nail art</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9n1gj</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1j9myrr</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Never thought I would be a 3D nail art kind of girl 🤭</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64883ip74aoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1j9mmip</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Press on question</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9mmip/press_on_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1j9mk4k</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>How can I repair my thin nails?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kposesn21aoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1j9mgt5</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Tips on applying full coverage tips on curved nails</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrhw3nrc0aoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1j9me40</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Supplement for Nail Health</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9me40/supplement_for_nail_health/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1j9lpex</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Did I go round/almond too early?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9lpex</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1j9lny4</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Polka Dot Nails for Spring 🩵🤎</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9lny4</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1j9lmhp</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>This lady seems to like my nails 🫠</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vc55nrhst9oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1j9lli9</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>im obsessed</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9lli9</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1j9kzgb</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Question: Glue to secure a dip</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j9kzgb/question_glue_to_secure_a_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1j9kplg</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Subtle seashell mani for my upcoming beach vacay!</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l5wvmlxtl9oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1j9kmfp</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>I used dried flowers in this set 🌸</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9st3lq2l9oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1ja6kyf</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>I think I finally got the hang of velvet nails!</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja6kyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1ja604s</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Repurposing polish brushes</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ja604s/repurposing_polish_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1ja5il0</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>ILNP First Purchase Advice</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja5i8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1ja55jz</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>4 days in</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ja55jz/4_days_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1ja5276</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>🌼!!Spring is Coming!! 🌼</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja5276</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1ja4cay</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Magnetic neodymium bars vs wands help</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ja4cay/magnetic_neodymium_bars_vs_wands_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1ja3ttc</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Mooncat’s Mercury in Retrograde</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1ie8qo7vdoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1ja38bg</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Requesting help finding a sheer light blue with green shimmer</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z92891t1pdoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1ja37qe</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Purple Amethyst Marble</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja37qe</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1ja2vg8</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>That's it y'all, I've made it!</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rf3yds7jldoe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1ja2tkv</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Best Polishes for Nail Art?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ja2tkv/best_polishes_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1ja29up</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Kbshimmer Haul: what should I try first?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpzkgodwfdoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1ja2644</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Goddess of Rot is so shifty!</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja2644</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1ja1z8e</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>BKL - Prince of Envy</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zgr10b5ddoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1ja1r33</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Fresh Mani!</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/toijx592bdoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1ja1pri</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>chrome isolation</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ja1pri/chrome_isolation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1ja1m6c</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Best jellies</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ja1m6c/best_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1ja1ita</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>I’ve just upgraded what I call “nail polish tower”</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja1ita</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1ja1g0z</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>St. Paddy's</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja1g0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1ja163z</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>How to achieve this?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmiobs4u5doe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1ja0yb4</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>I think I'll be throwing out my barry m peel it base coat</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gsk2xev3doe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1ja0udt</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Taking the cat eye trend literally</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja0udt</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1ja0k75</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Opinions on mainstream (?) brands?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ja0k75/opinions_on_mainstream_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1ja0hg4</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Colors between winter and spring ✨</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja0hg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1j9zo20</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Neon comparison</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9zo20</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1j9z9nt</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>deep red/maroon flaky top coat?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9z9nt/deep_redmaroon_flaky_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1j9z3wv</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Cracked - Mouse Ballerina</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9z3wv/cracked_mouse_ballerina/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1j9yz6n</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Darling Dahlia by Kokie Cosmetics💜</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9yz6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1j9yyvx</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>First attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9yyvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1j9yyql</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Jumping on the St Patrick's train</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cu1mfhdjmcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1j9y99d</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Pastels. For Spring. groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlvzh67ugcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1j9y4zo</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>we have cottagecore polishes at home 💅✨</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9y4zo</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1j9xlsz</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Love finding new combos with old favorites</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpb8851nbcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1j9xact</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Stockist list?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9xact/stockist_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1j9wzqa</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>KB Shimmer - do they hand-approve product reviews?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9wzqa/kb_shimmer_do_they_handapprove_product_reviews/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1j9wzll</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Serpents of Eden - Mooncat</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tm531dlu5coe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1j9w8su</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Are these the same polish? Yes, they are</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9w8su</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1j9vxbl</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Very pleased with this combo</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ggw9truhyboe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1j9vd3r</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>birthday nails 🥳</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9vd3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1j9v63g</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Day 1 vs. Day 14</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9v63g</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1j9ulmz</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Clionadh Psylocibin really does have an incredible shift of colors!</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9ulmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1j9u4km</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Batsquatch ft. Batman</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9u4km</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1j9tjvi</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Taking advantage of the recent sunshine with a little holo</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijjr53yvfboe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1j9tgnp</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Cetaceo</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmticym6fboe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1j9t7tm</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Dreamy Blurple Skittle 🫧🦋💜</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9t7tm</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1j9syfr</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Fiery attraction indeed</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9syfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1j9sxpt</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>How long does magnetic polish take to magnetize?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9sxpt/how_long_does_magnetic_polish_take_to_magnetize/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1j9swrb</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Emily de molly, what the heck.</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/036mr0n5bboe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1j9snwj</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Tired of Norpsilocin pictures yet? If so, skip this post.</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9snwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1j9scox</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>The lunula ombre mani has had a vice grip on me for over a decade</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xsq71p37boe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1j9sbj7</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>I couldn’t choose just one! Clionadh Cosmetics are lovely.</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9sbj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1j9rzh6</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Polish has lost its shimmer 😢</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jg5rpu6f4boe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1j9rufx</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>I need some vocab help? Let’s make a glossary!</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9rufx/i_need_some_vocab_help_lets_make_a_glossary/</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1j9rdiy</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Guess I am a holo-back girl</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9rdiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1j9rb8h</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Looking for dupes of DVN Abalone</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9rb8h/looking_for_dupes_of_dvn_abalone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1j9r47d</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Flight of the monarchs 🦋</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbksomfeyaoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1j9r06c</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>What was I made for?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9r06c</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1j9qud4</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>I'd like to get over 'I'm over it Rover' from Holo Taco</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9qud4/id_like_to_get_over_im_over_it_rover_from_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1j9qs0q</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>dupe for a defunct gap nail polish?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j57mgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1j9qi4h</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Had to try Maelstrom over black (thanks to posts here!)</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sn7jf2hrtaoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1j9q83y</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Bases for under Crelly/shimmers!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9q83y/bases_for_under_crellyshimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1j9q6bd</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Polish always peels off in sheets like 2 days after applying?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9q6bd/polish_always_peels_off_in_sheets_like_2_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1j9q637</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Dollar Deals - Sinful Colors</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ontfe6yhraoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1j9ovke</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>You can only order from 1 brand for the next year-what is it?</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9ovke/you_can_only_order_from_1_brand_for_the_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1j9ok5i</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Need to clean the edges but I’m in love</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9ok5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1j9odo9</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Which dazzle dry color is this?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwmpdxzmeaoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1j9nr9g</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>the EdM sparkle is actually unreal ✨</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9nr9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1j9myns</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>My press-on nail story (AKA looking for advice on painting, removing, repainting, and reusing press-on nails)</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>/r/lacqueristas/comments/1j9mt5n/my_presson_nail_story_aka_looking_for_advice_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1j9mykx</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Dark Pansy by Manucurist just replaced my favorite shade..</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3uiobm44aoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1j9mrks</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Glows in the shade, sun and dark</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9mrks</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1j9mojw</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Finally Home &amp; wearing my Party Hat 💗🥳</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9mojw</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1j9mjap</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Pretty in Purple</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9mjap</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1j9lwt1</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>OBSESSED with this cuticle oil pen</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nht0q7c6w9oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1j9lrrk</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Wild card: mixing magnetics</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9lrrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1j9lcva</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Sally Hansen Miracle Gel “Gel-ebration” 🍊🐱🥕🐹</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9lcva</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1j9l5b2</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Just what's needed</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9iiwe</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1j9jvp0</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Please suggest other polishes that are as glowy as Fair Isle (preferably purple/blue/blurple with different colored shifts like Fair Isle)</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0ucdd9qe9oe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1j9joo4</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Blinded!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w4pipfb0d9oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1j9j991</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>My most gel-like finish yet:  Lurid Lacquer's Riding Sleeping Bags Down The Stairs</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kigawu8v89oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1j9j950</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Zen by L.A Colors</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9j950</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1j9ifep</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Cuticula Top Coat really is worth the hype!</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9ifep</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1j8v9mo</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>[Gel allergy] Would reducing the frequency of getting gel nails help prevent me from developing a gel allergy?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j8v9mo/gel_allergy_would_reducing_the_frequency_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1j8vjiy</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>How do I use nail "stickers"?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j8vjiy/how_do_i_use_nail_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1j9djbm</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>What nail shape should I get?</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9djbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1j9hs28</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Lacquergram down ?</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9hs28/lacquergram_down/</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1j9hqa8</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Best CANADIAN peely basecoat, regular basecoat and quick dry top coat?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j9hqa8/best_canadian_peely_basecoat_regular_basecoat_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1j9hezj</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>My dream polish</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ispd09np8oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1j9hbko</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Heartbreaking news - A-England is officially closing</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9hbko</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1ja6gwy</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>lich nails 💀</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja6gwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1ja0ff5</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Maximalist celestial set for a client by me🤍</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja0ff5</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1ja1qws</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>chrome isolation</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ja1qws/chrome_isolation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1ja1a75</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Spring nail set with gel x from MG nail flushing</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8usbqtxs6doe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1ja158b</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Nail art I need to practice letters</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/betblm8m5doe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1ja0py0</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>FINALLY organized all my nail set (without buying anything new)</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja0py0</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1j9z21m</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>My cat-eye stained glass birthday nails! 🥳</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9z21m</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1j9yi8y</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>royally green press ons!!</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yftlj87xicoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1j9ye5s</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Structured clear french tips with irridescent foil</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9ye5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1j9xmra</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Some hello kitty wedding nails I made for a friend ^^</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0g7o96ubcoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1j9xiz9</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Pisces season ♓️</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9xiz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1j9waou</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Blooming spring 🌸</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlapl4qf1coe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1j9wa77</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>🐰Battle Bunny Miss Fortune🔫</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9wa77</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1j9vl9k</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>jellyfish press onss</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klkecdnwvboe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1j9o2vx</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>This week’s mani - not sure how I feel</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9o2vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1j9nfer</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>What do you use for 3D art?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j9nfer/what_do_you_use_for_3d_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1j9n765</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>First Set</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6x8xs5d06aoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1j9lmuf</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>I think I peaked, this is the best nail set I ever did yet, who would have thought yellow would be the one</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9lmuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1j9jedd</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Nothing beats a long vampy claw</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j9jedd</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1j9j1sq</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>New set 🐆</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vqftmr279oe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1j9iik4</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Nail Art by Husband For his Wife</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9skqh2l19oe1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Mar 14 08:11:16 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_16.xlsx
+++ b/data/collected_data/2025_03_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C897"/>
+  <dimension ref="A1:C1090"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15682,6 +15682,3287 @@
         </is>
       </c>
     </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1jaxwqk</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Ring finger is darker than the rest</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/warlnbn8sloe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1jaxl7i</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Keep this shape or go almond?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaxl7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1jawuq3</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Tiger Print nails + Cat eye polish</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xg9a8jsaeloe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1jawfcs</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Am i too dramatic if i go back to fix my nails in 6 days?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jawfcs/am_i_too_dramatic_if_i_go_back_to_fix_my_nails_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1jauowp</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>First time trying press-ons</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jauowp</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1jaujph</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Newest set 💙 swipe to see OG by u/looneylunime 🥰</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaujph</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1javv83</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Orange magnetic gel polish</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1javv83/orange_magnetic_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1javmby</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Why do I hate these so much?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zdc3n310loe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1jav0ud</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Pretty proud of these!!</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nya9pcwytkoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1jauz4c</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Holi Nail Hacks anyone???</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jauz4c/holi_nail_hacks_anyone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1jauw3l</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Is this normal :((( im worried</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jauw3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1jauvh3</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Nail cracking help?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jauvh3/nail_cracking_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1jaumlw</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>i love them but two gems already came off same day i left the salon. should i go back ? can they even fix that ?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmg5dyd1qkoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1jaqumq</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Now what</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9at37zdrjoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1jaubz6</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Yay spring</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaubz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1jas8ao</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>What should I do?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jas8ao</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1jatu4o</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Did I get overcharged?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmupwdwcikoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1jar9os</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>What supplies do i need to do my own nails as a beginner? credits: @bake.a.nail @setsbysuzy @siso.nail_j</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jar9os</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1jarhn2</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Did I choose tacky colors??</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jarhn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1jat2gg</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Help! I really suck at cat eyes 🤣😭</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jat2gg/help_i_really_suck_at_cat_eyes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1jatpue</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>So delicate, I love them</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnnp30u7hkoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1jatfqr</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Not much, but it’s honest work</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jatfqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1jat3sg</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Going for Poison Ivy vibes for the start of spring</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftuepdojbkoe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1jasr48</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Meow</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jasr48</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1jaspix</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Obsessed with my first builder gel set</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vaqqlhew7koe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1jascql</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>DND 2443 sheer sugar dupe?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jascql/dnd_2443_sheer_sugar_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1jas8e3</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Refill Set</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jas8e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1jas0ll</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>What’s your go to shape for the best press on nails?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jas0ll/whats_your_go_to_shape_for_the_best_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1jaruya</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Mocha ✨</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaruya</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1jaru0k</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Nail shape change after 8 years of coffin!</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaru0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1jars8g</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>If you do intricate nail art, consider a Macro Lens for the photos!</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jars8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1jarrhj</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Very pink 🩷😋🤭</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rv1u4hufzjoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1jarliq</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Builder gel advice</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jarliq</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1jaqr13</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Encapsulated fruit &amp; glitter</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaqr13</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1jaqqz0</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Shellac!</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl98xkgiqjoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1jaqn5d</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Fruity set🍊</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1mfy3x1npjoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1jaq9p9</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>How much do you tip ur nail girl?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jaq9p9/how_much_do_you_tip_ur_nail_girl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1japecq</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Latest Set vs Last Set</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1japecq</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1jaq0lf</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Beetles Cat Eye</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kh43tgobkjoe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1japql0</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>spring soot sprites 💕</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1japql0</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1jaowgb</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>First proper set I did on myself 💙</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ra4i479ibjoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1jaovpz</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Be so honest are these not it😭</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaovpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1jaoqw4</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Spring nails 🌸🌷</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62oru6saajoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1jaohz6</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>💜 Painted Polish Krewe Queen 💚 The perfect lavender for spring 🌱</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55ish1eb8joe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1jao1vx</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Pain in press on nails</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jao1vx/pain_in_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1jan4lj</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>My sister made DND inspired nails!</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jan4lj</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1jamv6y</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>does anyone know of any polish similar to this one?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88z1zsbpvioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1jaod4m</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>I just painted my nails with my new polish... what do you think of this color? 🌈💖</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/loatzy497joe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1jao9sy</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Builder gel chipping</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bd1m5o9i6joe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1jan436</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Midnight Nails🌑</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jan436</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1jamxj6</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>I know I’m not fantastic at doing my own nails, but I just adore this colour for spring. Featuring Poppy.</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqq10196wioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1jamp0y</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>New set. What do we think?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctdyrljeuioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1jalpbu</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Elegí un vestido azul eléctrico pero no sé si debería usar otro color random, que opinan?</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdcyiy6xmioe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1jales3</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Spring nails 🌷</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8yent5rkioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1jalars</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>St Patrick’s day? Shego? Cosmo? Idk but I’m in there🍀</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jalars</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1jakonp</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>I had one goal: get the tips ON. Everything else is bonus</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jakonp</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1jakgme</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Trialing a new shape as I wait for my other nails to grow.</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jakgme</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1jak3ru</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Will painting press ons with gel avoid an allergic reaction?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jak3ru/will_painting_press_ons_with_gel_avoid_an/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1jak83l</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oocaawztbioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1jajspx</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Inspo: Mountain Dew</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ad3fersn8ioe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1jajtn3</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Help! How to avoid a stain from leather boots on toenail polish?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jajtn3/help_how_to_avoid_a_stain_from_leather_boots_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1jajhkk</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>He said it’ll make it look less fat! Go back in or no</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jajhkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1jajhfn</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Reminds of robin blue eggs</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8s6sn9ub6ioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1jaj739</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Why can’t I ever get what I’m asking for??</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaj739</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1jaixr9</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Fresh set for Spring 🍀</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaixr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1jaiuo5</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>soak off after-effects?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oom2hjvp1ioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1jaj7tz</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>asked for a vampire vibe, couldn’t be more pleased !</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yifqavpc4ioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1jaj727</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Send help - addicted to the barbie pinks</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaj727</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1jairkr</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Saw some fishing lure nails here a while back and decided to give them a go!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybdr0l331ioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1jaip9a</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Do we like porcelain nails?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaip9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1jaifkx</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Natural Nail Growth Journey</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jaifkx/natural_nail_growth_journey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1jaihz4</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Pink!</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z246pwa4zhoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1jai36n</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Gel X Questions</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jai36n/gel_x_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1jai8o8</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Gel Press On Question</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vm1gdi89xhoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1jai77f</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>SECOND EVER MANICURE and it’s gorgeous</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jai77f</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1jahvli</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>How much would these cost me? I think I would need a tip put on.  Any recs in the south Jersey area? Nails by fresitaconcremita</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnsh6cujuhoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1jahfhh</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Reset my nails! Here they are with a layer of rubber base.</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fdzykrarhoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1jahcxv</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Organizing polishes without buying something new?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jahcxv/organizing_polishes_without_buying_something_new/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1jag4c8</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Name my nail salon...</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jag4c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1jagnts</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>My nails keep flaking -  give me advice.</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jagnts/my_nails_keep_flaking_give_me_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1jagfbe</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>I hate my new gel, pedicure color</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jagfbe/i_hate_my_new_gel_pedicure_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1jag93u</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Gel nail tips</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u27oczksihoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1jag8zt</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>What do you think of this design? I loved it to use it in March, the unicorn is kind of cute.</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y23ydywrihoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1jag6qi</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Look my Halloween nails did u like it?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykn39cmaihoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1jag003</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>First time ever, I could use some tips and tricks!</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jag003</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1jae26n</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Maybe I am overthinking it- Help would be appreciated!</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jae26n</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1jaey4j</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>First time doing Cat Eye for myself, but I'm  not sure I can see the cat eye. What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaey4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1jaez9y</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>St Patty’s Day Ready!!</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaez9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1jaexyd</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>What’s your favourite builder gel?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jaexyd/whats_your_favourite_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1jabpdg</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Thoughts on watercolour nail art?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jabpdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1jabaum</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>These crazy girls doing nails out of their houses are looking better and better ..</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jabaum</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1jaautg</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Am I bad at using nail polish or do my products suck?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jaautg/am_i_bad_at_using_nail_polish_or_do_my_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1ja9oko</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Nama Gel press on nails?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/namanailsltd?igsh=MXJnbmtrOWE2YnlkZw==</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1jaesqh</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Some of my recent work</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaesqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1jaei4y</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Super short press on</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jaei4y/super_short_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1jaemao</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>White is the best</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sde93n8m6hoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1jaej50</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>My weakness🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zr81qgvx5hoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1jaefdp</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Most shiny topcoat?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jaefdp/most_shiny_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1jaeawv</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Hard gel: building apex on shorties?</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaeawv</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1jae5sr</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>When the customs come out exactly how i imagined🥹💕</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jae5sr</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1jax7yi</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>BKL Immortality 💖</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtal0wo1jloe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1jawmzj</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Woow Starrily is beautiful! Northern Lights collection.</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jawmzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1jaubxi</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Shooting Star with my proteas looked so pretty this morning 🌷</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaubxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1jatlq7</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>What is the best shape of brush head, and why? What brand has the best brush to you?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jatlq7/what_is_the_best_shape_of_brush_head_and_why_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1jat58w</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Spring refresh for St. Patrick's Day</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jat58w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1jaslyx</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>How to get rid of dried blood &amp; repair cuticles after harsh cutting?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bh03rbz6koe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1jarts0</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Accidental Color Match</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bl5wx900koe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1jar6y6</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>ILNP Jelly Bean, but more lime green?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jar6y6/ilnp_jelly_bean_but_more_lime_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1jaqrb7</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Renaissance by Patty Lopes</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/31bmdndlqjoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1jaqrj2</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>I had an allergic reaction to the DND Gel lacquers that is similar to a gel polish reaction. If you also have a gel allergy, you may want to avoid these.</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaqrj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1jaql4r</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Chill Out</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jaql4r/chill_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1jaqj85</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>My problem trait trying to get rid of nail polish is that these are all different to me 😭</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1fbsb7oojoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1japvq7</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Crushing It for St. Patrick’s Day</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/deu5snp6jjoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1japht3</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Switching from gel to regular polish</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1japht3/switching_from_gel_to_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1jap42h</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Sunken treasure, my new favourite polish</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zksekvf5djoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1jaoh03</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>💜 Painted Polish Krewe Queen 💚 The perfect lavender for spring 🌱</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e179low38joe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1jao8b9</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>St Patrick's nails</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jao8b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1jao81w</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>$2.99 nail polish &gt;&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9ni6ru46joe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1jao1p7</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Horseshoe Magnet (ILNP, etc) vs 3D printed magnet for Velvet Nails</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jao1p7/horseshoe_magnet_ilnp_etc_vs_3d_printed_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1jans77</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Spring Skittle💚✨️🩷</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jans77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1janh1w</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Holo Jellybeans</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1janh1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1jane47</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>It’s raining and hailing but not in my apartment</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/todbxqipzioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1janakb</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>DIY nail decals with rhinestones? And also, acrylic paint in nail decals 🤔</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1janakb/diy_nail_decals_with_rhinestones_and_also_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1jan9kj</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Nail Newbie</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jan9kj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1jan1kf</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>velvetized forbidden fruit🍇🍏</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l2z4uw51xioe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1jamzyk</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Atomic Polish: Sour Apple Rings 🍏</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jamzyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1jamon6</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>naked sparkles ✨</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y5pbkp3buioe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1jammbp</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Forest Green + Shimmer what next?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jammbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1jam63x</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Kiss My Sass</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jam63x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1jalz2d</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Feeling kinda vampy with this polish 🧛🏿‍♂️</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f1d2nqnyoioe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1jaltbm</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Green nails for March 🍀</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaltbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1jakunp</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>S-melon like summer 🍈✨</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jakunp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1jajpc0</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Blurple (blinkle?) skittle on a new nail shape</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qr2xa8a08ioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1jaj0tg</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Decided to combine my love of nail polish with my love of crochet!</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s732f57o1ioe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1jaiyam</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Linkin Park Nails</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i29lz80g2ioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1jais3z</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Help me identify these opi cuties?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jais3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1jaiitv</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>ILNP - Eclipse</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaiitv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1jaihgm</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>My nail art with magnetics (all regular polishes)</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/olrn2tmjyhoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1jaibi8</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>I Am an Appetite (BKL) &amp; The Sink After He Shaves (DVN)</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/btzd18zsxhoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1jaib41</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Shimmer Goodness!</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaib41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1jai4xt</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Organizing polishes without buying something new?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>/r/Nails/comments/1jahcxv/organizing_polishes_without_buying_something_new/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1jai1l3</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Polished for days - Salamándra 🦎🔥💙</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4o55mxdrvhoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1jahz5q</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>UK oil recommendations?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jahz5q/uk_oil_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1jahyux</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Spring Bling! 🍀</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jahyux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1jahvy1</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>rainbow gemstones 🌈 💎</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iia6i65muhoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1jahh9e</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>not exactly a spring color, but I had to test that glow 🌟</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jahh9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1jahcjh</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Seven Sins</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jahcjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1jaha16</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>when your nails match your hair…</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaha16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1jah1hn</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Black and White Floral</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jah1hn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1jagzma</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Do you believe in magic?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jagzma</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1jagqbg</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>💘</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k64fo5hcmhoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1jafo9h</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Pretty Shorties - Emily de Molly Guiding Light</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jafo9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1jaffj6</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>What is my purpose?</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6ioj61pchoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1jaf6tj</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>ILNP Deep Space</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tj6psgxtahoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1jaevu8</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Franken polish information</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jaevu8/franken_polish_information/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1jaegkf</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>My oldest polish</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v40dfjme5hoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1jady7o</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>My polish setup!</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49jtz9rj1hoe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1jadlcq</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Mermaid</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jadlcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1jad6fc</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Please Help!!!m</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jad6fc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1jad5qu</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Oceanic Nails</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q5et9odavgoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1jacy6s</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Time for some green!</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jacy6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1jacgh7</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>First time getting gels done</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jacgh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1jacbft</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Gel X with air dry lacquer?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jacbft/gel_x_with_air_dry_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1jac6pm</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Stick pic 18+ 🥵</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lu50zcu9ngoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1jabtr2</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>🫒Olive It!🫒</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jabtr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1jabbkq</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>How do I fix my nail beds and cuticles?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jabbkq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1jab9y0</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Cracked: Please help me whittle down my cart</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jab9y0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1jaaui2</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>The Power of Fantasy💜❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jaaui2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1jaa3en</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Greens for March 💚</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jd6lyc3d3goe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ja3fgj</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>OPI - Needle in a Haystack dupe?</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ja3fgj/opi_needle_in_a_haystack_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ja8tma</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Can some one tell me what this is??</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7wfdhcoofoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ja967b</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Twinkled T swatches</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ja967b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ja84pv</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Help me pick my wedding day polish(es)?</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivu9l74uffoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1jayuyc</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>What do you think about this?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3n52p65j4moe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1jayux1</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>What do you think about this?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o62hh3ki4moe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1javvpy</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Some of my work.💅🏻</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69liozat2loe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1jasc8v</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Can I leave projects unfinished?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jasc8v/can_i_leave_projects_unfinished/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1jar3lu</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Randomly cohesive?</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jar3lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1japw4w</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Redbull - a salon workers holy grail 😆🪽</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqq5gndajjoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1japg4y</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>2010 meme nails</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1japg4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1japeqr</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Manzanilla olives</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k79nowkhfjoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1janstp</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>3D sculpting gel not fully curing? Normal? Recommendations?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1janstp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1jals8p</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Bandi Aurora Glaze nails ✨</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/512tvj4fnioe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1jalou8</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Custom press-on order</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jalou8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1jakddu</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>One of the best nails you will ever see in your life.</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ly0pmgxcioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1jajoy6</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Spicy gurl 🌶️</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eep95suw7ioe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1jai7vv</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Painting Special effects</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jai7vv/painting_special_effects/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1jahmma</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>My nails</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8ghz5uaqshoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1jag4ws</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Plaided and cute!!</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jag4ws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1jacvn9</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Dark red press ons!!</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clddpyv0tgoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1jach3w</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Some of my recent work ❤️ I love designing nails</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jach3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1jacce3</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Celestial nails</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y55up84kogoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1jabajx</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Small line details tips?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjl47sacfgoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Mar 15 08:09:38 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_16.xlsx
+++ b/data/collected_data/2025_03_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1090"/>
+  <dimension ref="A1:C1301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18963,6 +18963,3593 @@
         </is>
       </c>
     </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1jbpjnt</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>boyfriend picked the colour and shape</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mjuzm64zsoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1jbpj3x</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Fitness and Nails are on point</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tiqnl62zsoe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1jbpdm6</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Spring nails with cow print.</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbpdm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1jbp8co</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Nothing stays on my nails</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbp8co/nothing_stays_on_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1jbnr48</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Ridiculously unhappy with gel french manicure (nails before manicure and after)</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbnr48</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1jbmq4q</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Question about acrylic shape</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbmq4q/question_about_acrylic_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1jbmoai</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Ultimate beginner advice</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbmoai/ultimate_beginner_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1jbhwjz</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Do my nails look immature?</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbhwjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1jbo9zh</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Newbie progress</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbo9zh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1jbo8rf</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Just brought a dress this color, what nail color would go best with this?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3ecth4pisoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1jbnsir</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>At home nail product recs??</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbnsir/at_home_nail_product_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1jbn53c</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>What are these dark spots on my nails?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbn53c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1jbmsew</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>first acrylic set at home!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbmsew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1jbmb8c</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Nail day is the best day! Obsessed 🤩</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbmb8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1jbivf3</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>What to expect from first biab mani? Should I just stick to regular gel?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbivf3/what_to_expect_from_first_biab_mani_should_i_just/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1jbil00</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Need spring nail inspo pics for my next appointment.</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbil00/need_spring_nail_inspo_pics_for_my_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1jbenbb</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>New set today, I've had the inspo Pic saved for months and finally got to do it! Apres Gel X</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbenbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1jbi92f</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Any natural nail girlies that have a mild case of Symmetry OCD with a hint of perfectionism. How do you come to terms with how nail looks? Shaping them, painting them, designing them. How do you make peace with them?</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbi92f/any_natural_nail_girlies_that_have_a_mild_case_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1jbjw3i</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>First two tries painting nails</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbjw3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1jbfnp6</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Does anyone know why my gel nails are wearing down/staining like this?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuewhecz9qoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1jbj5jh</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Cruelty Free OPI Dupe</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbj5jh/cruelty_free_opi_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1jbjo6b</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Nail recommendations</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jw0zsumt7roe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1jbl3ho</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>NEED HELP FINDING THESE KISS PRESS ON NAILS!</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbl3ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1jbkwd1</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>New to Acrylics - Is this About Normal?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbkwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1jbm46i</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Does this shape/color suit me or should I change?</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lan27a3vroe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1jblrt0</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>I tried Jade for my March green nail month</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jblrt0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1jblxyo</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Please critique!</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vaitehmdtroe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1jblr6e</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>I love long nails but they’re expensive</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jblr6e/i_love_long_nails_but_theyre_expensive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1jblnsj</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Polygel</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jblnsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1jbllps</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>First ever manicure - Gel X</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbllps</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1jblcir</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Attempting to do my own nails, how did i do?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jblcir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1jblaaw</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>A cute DIY spring set 💐</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jblaaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1jbl6h0</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>What do you think of nails over last 6 months</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgrw52lulroe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1jbl58w</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Nail Prices</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbl58w/nail_prices/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1jbks51</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>my nail tech’s work from my newest set to my first set with her</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbks51</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1jbkrb9</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Put on some press-ons just because. Feeling pretty, but now I gotta remember how to function with these.</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbkrb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1jbkm36</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>My mom copied my nails and HAD to one up me with her flower design</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbkm36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1jbkkxt</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Spring is right around the corner. Here are some of my favorite spring sets I've done so far 😊</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbkkxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1jbkks3</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>glassy rosies 🌹</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63uzx7o7groe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1jbkhvt</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Where can I order some great press on Nails?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbkhvt/where_can_i_order_some_great_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1jbjz4z</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Coral and silver glitter gelish, do we love it?</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbjz4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1jbjy8v</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>I painted them myself at home, what do you think? 🌈💅🏼</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqzovinearoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1jbjw42</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Birthday nails 😊</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbjw42</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1jbjry3</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Perfect Pinkish White Dip Powder</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbjry3/perfect_pinkish_white_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1jbjh9q</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Moon nails 🌝</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbjh9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1jbizv9</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Waiting for Spring 🌸</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yiiu2gtq1roe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1jbiroo</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Can I use arts and craft gold chrome on nails?</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbiroo/can_i_use_arts_and_craft_gold_chrome_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1jbie1r</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cn2eafhwqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1jbidp6</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>nail day 💕 price?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbidp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1jbiam0</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Fun with patterns</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x82c5g7kvqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1jbi6hj</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Didn’t get a good pic but I had fun utilizing my free will on these</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7uxmkmruqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1jbi443</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Paying tribute to sleep token and St Patrick’s Day is</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbi443</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1jbi0fd</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Thoughts on this color??</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbi0fd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1jbgd55</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>✨Ethereal Vibes✨</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbgd55</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1jbhi3n</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Newest Nails!!</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbhi3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1jbhrf9</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Gel-X looking too wide/bulgy</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbhrf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1jbhqs8</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Did some Sonic nails</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbhqs8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1jbhjlo</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Is this shape okay?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbhjlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1jbh9lx</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Strawberry Glaze on Natural Nail (I believe it's hybrid gel)</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbh9lx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1jbh6yk</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>I love this color 💜</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zs13c6xfmqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1jbgxym</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Love my nail tech! Ready for spring!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbgxym</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1jbguzy</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Improvement?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbguzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1jbgtjn</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>thankyou mother! (ft gecko)</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbgtjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1jbghnq</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Which color combo for my next set?</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br5bopwmgqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1jbfzlv</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Bejeweled</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwp8wsjncqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1jbfxwl</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Galaxy glitter encapsulation</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6k548r9cqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1jbfs1i</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>I’m in love!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3f6plpqyaqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1jbfp3x</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>is this supposed to happen?? (the nail polish being visible through the bottom)</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wz6jby0aqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1jbfnyh</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Ready for the Dominican Republic! 🏝️🇩🇴🐚</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbfnyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1jbfimg</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Red nails in corporate?</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bilzdz6v8qoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1jbfaer</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbfaer</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1jbf6r2</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Back in business after 2-3 month break💅🏼</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmtnv1tb6qoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1jbf5ig</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>St. Patrick's Day design</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7luio826qoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1jbewi7</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbewi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1jbennh</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Top pink??</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ua88z4972qoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1jben8w</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>First sets of nails</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jben8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1jbed5p</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Pink &amp; Green Magical Set 🩷💚</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/410yw7rvzpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1jbe8v9</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>What service should I be booking?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbe8v9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1jbe79j</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Acrylic nail cracked slightly?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3oxqvonypoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1jbe6c8</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>HELP!! NAILS TOO SHARP</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvtcfmdfypoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1jbdaji</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Really awkward hands/nails…  How did she do?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbdaji</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1jbdnpg</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>My recent nail designs</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbdnpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1jbdltr</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>My marble work.</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4z9j30zztpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1jbdep6</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Press ons are a game changer</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbdep6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1jbdcfs</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Advice on my nails?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73p5jrt0spoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1jbd2v3</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Press On Nails</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbd2v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1jbczu2</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>bleeding reverence 🗡️🩸🗡️</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbczu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1jbcun0</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>I tried doing chrome on chrome fruits &amp; other hand is watercolor fruits 🥰</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/hZ3vzSD</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1jbcnyb</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88gkulexmpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1jbcith</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Koi pond (ft frog pond)</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbcith</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1jbceky</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Short nude and butterflies</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbceky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1jbc61x</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>how to not get water trapped under press ons?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jbc61x/how_to_not_get_water_trapped_under_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1jb8rsk</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Growth</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb8rsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1jb95oy</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>dual form nails</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i95uuq20vooe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1jb9obo</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>First attempt at natural stone nails!</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb9obo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1jbc33x</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Pink frenchies are my spring/summer favorite 💞</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbc33x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1jbc0zu</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>To say that I’m obsessed is understatement</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbc0zu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1jbc0ak</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>A spring pastel set 🌷</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9d1zyafwhpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1jbb4hm</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Nail school test set</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gjw42yecbpoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1jbarpt</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Me time</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2usrdlp8poe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1jbq2hi</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Cool toned transparent light nude</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8rckm986toe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1jbp9m4</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Press ons on curved down nails?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jbp9m4/press_ons_on_curved_down_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1jbosue</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>I asked this subreddit to help me ID her and now here she is :)</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbosue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1jboczw</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>baby’s first velvet</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w8ktjt25ksoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1jbnxqx</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>So upset</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/im9pznx3fsoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1jbnwxg</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>In light of the recent tariffs, can we make a master list of non-US-based polish makers for our Canadian lacqueristas?</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jbnwxg/in_light_of_the_recent_tariffs_can_we_make_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1jbno90</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Okay I've been sleeping on Alchemy Lacquers because it's breathtakinggg</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbno90</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1jbnfii</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Lurid + ILNP = 🥰</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbnfii</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1jbn7up</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Polished for days- enchanted to meet you 🩵</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbn7up</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1jbn3av</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Finally inked my polish dice!</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3ez5qqyr5soe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1jbmzh7</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce : Quid Pro Quo</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbmzh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1jbmmcz</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>My St. Patrick's Day Green 💚</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yqqkya7j0soe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1jbmia4</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce - Ignite the Spark</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbmia4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1jbmf3k</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Smooooth</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbmf3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1jbma8e</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Green &amp; Gold(yellow) Skittle for this weekend!</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i58z8x41xroe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1jbm9yu</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>I have a horrible nail biting habit so I don’t paint my own nails but my standard poodle doesn’t mind it. 🩷 Little watermelon French tips and they came out so cute. (Dog safe nail polish)</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbm9yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1jbm6tr</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>the stolen kiss</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qammpn7svroe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1jblmyg</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>I love jelly polish but haaaate a visible nail line.</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jblmyg/i_love_jelly_polish_but_haaaate_a_visible_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1jblis4</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>I love the way this light pink is shimmering such a bright white. Are there any similar colors out there?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5od7hi5aproe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1jblgk3</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Swimming in the Ocean Blue</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vhhzlhaooroe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1jbl2dn</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>My St Paddy mani!</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbl2dn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1jbku9y</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>help me find the taup/brown/purple</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0dee45oiroe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1jbkbe4</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Anyone else smell their nails to see if they’re dry yet?</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jbkbe4/anyone_else_smell_their_nails_to_see_if_theyre/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1jbkaqo</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Salon perfect make it flashy</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbkaqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1jbk72i</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Mardi Gras - to - St. Patrick’s Day mani. Day 9 and still going strong! 🍀💅🏻💪</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uf4dd6u7croe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1jbk5dq</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>St. Paddy’s Day mani ☘️🌈</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbk5dq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1jbjece</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>feb ppu order came in 💜💎</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbjece</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1jbjb8m</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Juicy Green Mani</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbjb8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1jbjb2k</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Juicy Green Mani</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbjb2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1jbixfr</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Canadian nail polish brands</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jbixfr/canadian_nail_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1jbipp8</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Cuticle/proximal nail fold issue?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbipp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1jbiljs</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Baby Billy’s Bible Bonkers</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbiljs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1jbihto</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Digging through my old polishes and found this gem</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynsbpq7exqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1jbi6sf</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Newbie</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xw1j7m0uuqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1jbi44d</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>st. patrick’s day mani!</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ecs7c07uqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1jbhur0</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>random but free nail polish haul !</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbhur0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1jbhe7j</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Long time lurker, first time poster</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbhe7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1jbgu4r</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>WWDITS Stardust Shimmer Collab</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jbgu4r/wwdits_stardust_shimmer_collab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1jbgjyy</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Anthropologie icon juice glass nails 💅 🤓</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbgjyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1jbgjgq</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Dear Santa.. in the middle of March 🤣❤️</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbgjgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1jbgbbj</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Cheers to Good Fortune!</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbgbbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1jbfu4h</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Replacement for glossy taco top coat that's not American</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/483dkbsfbqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1jbft7h</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Where can I find a polish closest to this color?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qabmm1d8bqoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1jbflph</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Happy St. Patrick's day!</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbflph</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1jbfjml</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>RIP Snowstorm mani — took down my tree, took out my nails.</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbfjml</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1jbf96u</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>DVN: What am I missing?</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jbf96u/dvn_what_am_i_missing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1jbf667</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Beautieus Pluteus</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hpvs48b66qoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1jbesqb</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Velvet nails…</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/djju93z93qoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1jbdzjm</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>New wagnet holder DIY</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ht2x0mywpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1jbd4e2</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Does anyone know where i can find a polish the same color as the pink in this photo?</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwwv06cbqpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1jbdl3r</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Feels like most people go with almond or oval. Who else prefer square?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kh0h17sutpoe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1jbdc8l</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>happy st patrick’s day! hand painted by me (__kmnails)</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsk3u8azrpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1jbd8ws</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>I think I know what I’m wearing to my astrophysics PhD defense 🌌 ✨</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4jqjj2x7rpoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1jbcqjc</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Every time I think I’ve found my perfect warm clay red, it ends up pink😆🌷</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q68fgvahnpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1jbcpsu</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Nailbed pain :((</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jbcpsu/nailbed_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1jbcd9z</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>I couldn’t choose a green so… I didn’t 🍀</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbcd9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1jbbzk8</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>My friend helped me put my shelves up. My husband think this is a lot of nail polish… 😂prove him wrong</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ilrl4gmthpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1jbbt22</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>new favorite color 😍</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbbt22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1jbbffn</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>If nails could scream “We’re ready for spring!”</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbbffn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1jbb66u</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Oooohhh shiny</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fy0fvtbobpoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1jbagu9</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>I Smile at Your Footfall</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbagu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1jbafnq</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ta9f3t06poe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1jb9ylo</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>LynBDesigns new release benefits conservation! Also they’re having a 50% off sale!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb9ylo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1jb9vxx</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Sage 🌱</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb9vxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1jb9vjs</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Had to cut my nails because one broke and then got my nails done for the first time in 5 years Had no idea shorties could be so cute!</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb9vjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1jb9s40</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>What to expect from a BIAB manicure?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jb9s40/what_to_expect_from_a_biab_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1jb97oe</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Learning how to do my nails</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb97oe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1jb8jt6</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Happy St Patty's weekend!</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb8jt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1jb8i22</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Chrome trial</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92hw6q19qooe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1jb84wz</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Peeling?</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb84wz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1jb7n8v</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>please recommend me more polishes to wear to the club!</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb7n8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1jb7klz</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Do any brands sell swatches?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jb7klz/do_any_brands_sell_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1jb7cup</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Spring Break Vibes</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb7cup</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1jb7are</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Brace for the Fallout</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb7are</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1jb6xm5</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Keeping it simple this St. Patrick’s 🍀</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ryw6q2ceooe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1jb61h1</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Does Anyone Else Think the New MC Reward Looks Like ILNP Rosewater?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jb61h1/does_anyone_else_think_the_new_mc_reward_looks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1jb5t66</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Top row is Mooncat, bottom is ILNP. I think I have a blurple problem lol</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zjpkkk3s5ooe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1jb5lkw</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>How many nail polishes do you own?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jb5lkw/how_many_nail_polishes_do_you_own/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1jb59ko</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Help me pick my St Patrick’s day polish</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7iv90dhh1ooe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1jb52mv</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>European indie brands?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jb52mv/european_indie_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1jb4xal</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Left Your Text On Red by OPI on natural nails 🔥📵</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb4xal</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1jb48px</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Does Bluebird Lacquer send emails?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jb48px/does_bluebird_lacquer_send_emails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1jb3xbs</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Holo Taco - Milky White Shimmer (and some stamping)</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb3xbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1jb3s4p</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Tell me you’re the most beautiful polish without telling me. 😍</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gj9p1uh3pnoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1jb3egq</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>3d clouds jelly nails</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb3egq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1jb36qe</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>OPI - Just a Hint of Pearl Pie</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb36qe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1jb34xw</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Happy Pi Day! 🥧</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb34xw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1jb0xo3</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Deep Space 🌌 ✨</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w14nz6g6wmoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1jaoy12</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>So late to the velvet trend</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q5idxvnubjoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1jatdbs</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>I love purple</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ebvz7zc0ekoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1jbhr5s</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Isolation Chrome 3d Designs</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/nKulI0u_CnA?si=4sP86JOpWqPzH69v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1jbhr4r</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Did some Sonic nails</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbhr4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1jbflfv</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Mushroom butterfly nails! 🍄🦋</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iiibudci9qoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1jbetwd</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Fruit nails😋</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c88idu8k3qoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1jbebjw</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Press ons I did</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbebjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1jbe11v</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mthap8axpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1jbdwbs</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Been doing nails for 2 years now but only recently decided to start doing designs</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwkm6z9awpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1jbdkyo</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Glitch effect attempt</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apapabbttpoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1jbcw34</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>bleeding reverence set 🗡️🩸🗡️</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbcw34</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1jbc9v3</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>New Set.</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbc9v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1jb9kbm</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Nailz_by_dev</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jb9kbm/nailz_by_dev/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1jb8gn7</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>swan Lake</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0t8iuqypooe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1jb6sz4</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>I would KILL for nails like these.</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb6sz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1jb5h9c</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>The nails my sister wanted me to do for her</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4boc93563ooe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1jb52eg</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>If anyone can make press on nails like this please hmu 😊</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jb52eg/if_anyone_can_make_press_on_nails_like_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1jb4gse</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>gel questions</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jb4gse/gel_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1jb4bnq</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Good morning✨ ready for Easter ✨ how did i do it?</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0abxm55stnoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1jb0lyb</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Eyeball nails</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jb0lyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1jb08pl</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Wee little dinosaurs 🦕 🦖</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvagr93dnmoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1jb03hx</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>tried butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/erfw5ceelmoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1jayz8t</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>First time practicing detailed nail art 😇</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jayz8t</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Mar 16 08:10:07 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_16.xlsx
+++ b/data/collected_data/2025_03_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1301"/>
+  <dimension ref="A1:C1489"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22550,6 +22550,3202 @@
         </is>
       </c>
     </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1jcgmcb</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>I'm back to being OBSESSED with pink 💕🫧</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrjzjd3jd0pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1jcgkod</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>St Paddy’s Day/Springtime mani</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcgkod</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1jcg62w</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Is it better to have gels on natural nails or acrylics?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jcg62w/is_it_better_to_have_gels_on_natural_nails_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1jcfqgg</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Green n white chrome?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcfqgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1jcfzq2</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Pop out in pink</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcfzq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1jcfzlu</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Tried new press ons</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ww7ne7u40pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1jcflza</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Spring picnic nails</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcflza</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1jcebxx</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>How often do you need to fully remove hard gel?</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jcebxx/how_often_do_you_need_to_fully_remove_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1jcebp6</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>What shape would look best?</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j357wztijzoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1jce5xi</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Spring set!</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u20yeq6ohzoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1jcdx8i</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Pretty with Pink</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvrwlg6wezoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1jcdvdl</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Normal Outcome? Bulky Dipped Nails</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcdvdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1jcdszf</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>What is a reasonable price for this Gel-X set?</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myx4rz8jdzoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1jcbhaw</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Nails from Winter</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aa0ndcbcpyoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1jccyzd</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Nail Gems Fix</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jccyzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1jccw8o</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Question about lots of stuff. (Been trying to grow nails for 3 years.)</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jccw8o/question_about_lots_of_stuff_been_trying_to_grow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1jcbxzb</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Press on nails longer than 45 mm?</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jcbxzb/press_on_nails_longer_than_45_mm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1jcb4vx</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Don’t mind me, I’m OBSESSED</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcb4vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1jcb29r</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>chipping at free edge</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jcb29r/chipping_at_free_edge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1jcamv6</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Too long for this wedding?</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcamv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1jcajly</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>help! bubbles under a few of my natural nails??</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aa76ezkbgyoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1jc8pxp</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Russian Manicure + long term travel ( 2 mos)</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ox4oyvmzxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1jcdjof</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>French dragonfruit</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58zz9p1nazoe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1jcdj8q</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Classic French</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcdj8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1jcdabo</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Spring!!</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcdabo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1jcczp3</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>spring has sprung ! ☀️🐝 (almost)</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qi1q03np4zoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1jccx4h</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Press-on Set I made for a friend</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jccx4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1jccpow</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>New Set 🍀🦓</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e91lmitq1zoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1jccggc</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Please help</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jccggc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1jccg76</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Tried cat eye and chrome powder … girlllll</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jccg76</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1jccdzg</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Nail dip powder</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jccdzg/nail_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1jccchf</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>St. Paddy's Day Nails</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jccchf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1jcc45r</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>new nails!!!</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcc45r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1jcby4e</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>New set &amp; New to getting designs and I’m very happy</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcby4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1jcbx3x</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>St. Patrick's Day Nails 🍀☘️🍀</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcbx3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1jcbtb1</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>went simpler this time!</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4yslpqmsyoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1jcbgr9</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>St. Patty’s day nails 🍀</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcbgr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1jcbbc9</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Is my nail ruined?</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcbbc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1jcar27</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Spring nails!</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gd7j5o8iyoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1jcanch</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Green nails for St Patty’s day ☘️</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcanch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1jca6xc</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>New to acrylics.. Is this normal?</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jca6xc/new_to_acrylics_is_this_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1jc6aff</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>rubber base staining</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60xh2xilexoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1jc72lc</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>How do you find a nail tech in England?</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jc72lc/how_do_you_find_a_nail_tech_in_england/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1jc87cv</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Techniques to achieve this look besides free-hand? art by @nailhavenct on ig</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc87cv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1jca857</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Fresh nails make me wanna slap someone</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bcmneebdyoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1jc94oy</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Salon ruined my nails</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6s7vu6t83yoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1jc9x8j</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>New to Acrylics - Is this Normal??</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc9x8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1jc9xcl</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b38i58piayoe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1jc9x4l</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Chrome over natural pink</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc9x4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1jc9nno</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Spring ready</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1xjknvy7yoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1jc9mh9</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>My new set, im in awe</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0l0y15o7yoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1jc9isb</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Do I have to use builder gel?</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jc9isb/do_i_have_to_use_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1jc9iq6</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>I had no plan and my nail tech still made a piece of art😭🩷 (I’m obsessed with gemstones😂)</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc9iq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1jc9hhm</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Nobody believes they are my natural nails</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/noe3mfwe6yoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1jc9d2q</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Reporting from the future because that’s where my nail tech is from</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ln5mxlb5yoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1jc8r39</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>NANA nails i did today 🖤🩷</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1a28q5hwzxoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1jc8llm</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Did my own nails for the first time in a long time</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14hcm4ojyxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1jc8kx6</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>It took me 7 hours</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9irswrdyxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1jc8ja1</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Another press on set</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipoodfazxxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1jc895r</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Rate my friends nails - I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zqr7mdivxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1jc6ck8</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>My nails I did today, inspired by a bowling alley carpet🫡</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sj238423fxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1jc82hv</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>I did this set today 🌷</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdl2k8svtxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1jc7pc1</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Erin go Bragh! ☘️</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ehoua8pqxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1jc7fbt</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>I think I might have made the most niche nails ever</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc7fbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1jc78ue</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exk5qjqrmxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1jc762i</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Said I wanted simple purple and spring</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yo08ee3mxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1jc6cvp</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Sparkly purple on natural nails</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzl5wjw5fxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1jc6ck9</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>My nail tech absolutely ate down once again</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc6ck9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1jc69pm</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Nails smell like chemicals after manicure</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjp2macgexoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1jc5w41</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Where can I find a polish closest to this color?</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jc5w41/where_can_i_find_a_polish_closest_to_this_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1jc5nla</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>New witchy nails</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69mdu32n8xoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1jc5fjo</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Need Spring nail inspo pics please</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezkuozgs6xoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1jc5h4r</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Talk to the hand cause the face ain’t listening 🤭</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc5h4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1jc3zw4</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Canadian Shellac Polish Brands?</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jc3zw4/canadian_shellac_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1jc593n</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>I attempted the clear tips with builder gel</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlfew81b5xoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1jc566g</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>my care bear waterslide frenchies 🥹</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mif5wkpm4xoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1jc548h</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Biab</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc548h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1jc521l</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Did my moms nails</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/py5456zp3xoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1jc520c</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Amazing Cat Eye!!</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhpladtp3xoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1jc4vxe</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>I'm delighted with my nails ❤️. My friend is the best</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc4vxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1jc4v4e</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Neon green!</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc4v4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1jc4jfc</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>I'm so proud of my new set. and it's first time do my foot nail by myself.</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc4jfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1jc4iwv</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Did I get hustled at the nail salon?</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xuezqzczwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1jc4h4s</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>my birthday nails! Love this shape 🍀💚</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwua5anyywoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1jc4d8t</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>The nails I need SOON</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc4d8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1jc4bv1</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Nipper or cheap e-file for excess/tough skin around the nail. Personal, not for professional nail care</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jc4bv1/nipper_or_cheap_efile_for_excesstough_skin_around/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1jc4an7</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Short gel manicure on natural nails</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2ef6b4ixwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1jc4380</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Did a springy set for my brother-in-law’s girlfriend</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc4380</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1jc41m3</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Which shape looks better?</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc41m3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1jc3wbr</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Bows, frogs and mushrooms. I’m in love</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc3wbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1jc3s9y</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Pretty new to the nail game and I’m obsessed with this polish I got</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pq3w77mftwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1jc3pnm</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Purple Aura</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5pmbaowswoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1jc3jnj</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Gel Polishes for Press on Nails</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jc3jnj/gel_polishes_for_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1jc3foh</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Bright and cheerful 😌</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llz64c9pqwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1jc375g</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Like A Ross nail set</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65cu4w6qowoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1jc369l</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>I call these “june bug nails”</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbst8nojowoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1jc2yq3</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Cottagecore Nails</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oinelupwmwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1jc2u6a</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Jujutsu Kaisen Sukuna nails</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38kpt07wlwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1jc2s9p</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>First time going to a new nail person in years</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc2s9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1jc2oub</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Does getting cat eyes add cost?</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jc2oub/does_getting_cat_eyes_add_cost/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1jcg53r</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Christmas vibes 🎄</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ih251tay60pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1jcfcip</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Green blue mooncat skittle</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/237prxjcwzoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1jcf73t</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Magnetic jelly sandwich time 🧲</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcf73t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1jces2b</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Couldn’t decide on a green for Paddy’s day so I did them all.</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ns1s4h16pzoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1jce8vc</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Lost Berry vs. Merlot</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jce8vc/lost_berry_vs_merlot/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1jce49h</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Wedding Nails Potential</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4tem7057hzoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1jcdq9x</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Am I the only one who hates the Essie Gel Couture Top Coat's bottle?</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56rqp51oczoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1jcdn1v</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Clionadh Psilocybin and Psilo sibs!</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5wttodiobzoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1jcd7yw</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Abstract hexcore inspired nail art!</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcd7yw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1jccmfd</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Cracked — Cupid Missed</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jccmfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1jcc8ak</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>First time using press on 💅 and used LA Colors polish to try them out!</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/locjawrqwyoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1jcc7nr</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>gorgons gaze 👁️👄👁️</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcc7nr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1jcbxkg</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>St Patrick’s mani 🍀🌈</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oysto3fttyoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1jcbrxh</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>LynBDesigns Spill the Teal vs. ILNP Retro Teal?</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jcbrxh/lynbdesigns_spill_the_teal_vs_ilnp_retro_teal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1jcbo4u</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>St. Patrick's Day Mani - Every Single Green Polish I own</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcbo4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1jcbfhr</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Sparkly nude of my dreams</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4ygais0uoyoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1jcbamk</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Manicure case?</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsa3a1xhnyoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1jcb61q</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Love Reading by BKL 📖 💚</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcb61q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1jcawx9</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>St. Patrick’s Day Mani</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcawx9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1jcathf</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>The back up bottle.</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jcathf/the_back_up_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1jca6fn</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Lacquer releasing a new line on March 25 (unaffiliated)</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jca6fn/bees_knees_lacquer_releasing_a_new_line_on_march/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1jc9q71</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Current mani and today’s Dollar Tree haul</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc9q71</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1jc94iu</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Tried a look</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sc1o0da73yoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1jc8wiv</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Party Punch by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/81771iw61yoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1jc8vyl</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>OPI Chasing Rainbows</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97xmfzc21yoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1jc8umd</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Lots of celestial activity happening in the sky lately 🪐⭐️🌘</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc8umd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1jc8ac5</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>Storage solutions</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc8ac5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1jc8065</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Amazing service from Cracked</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jc8065/amazing_service_from_cracked/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1jc7yn9</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Looking for a “clean” alternative to Pink Armor Nail Gel</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc7yn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1jc7xg4</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Renaissance</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1upmkcqlsxoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1jc7lgq</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Pink or Swim &amp; Flower Child</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6qqrljrpxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1jc75kg</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Techniques to achieve this look besides free-hand?</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc75kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1jc6vcd</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>sally hansen GKP carrot cake</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ku9ytfikjxoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1jc6q16</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Strawberry Skittle!</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6knoojaixoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1jc6es8</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>First ILNP Order</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc6es8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1jc5eq3</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Spring is in the air!</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awupzqbl6xoe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1jc5b9t</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Aloha Kitty</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc5b9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1jc51yr</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Transparent 💚</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc51yr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1jc41ss</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Holo Taco collection ID?</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3oq6xhivwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1jc3q2d</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>No magnetic polish in store?</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jc3q2d/no_magnetic_polish_in_store/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1jc3m7c</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>The juice is loooooose</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvzi98v4swoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1jc3h3u</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Mooncat Maelstrom really is THAT girl</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pnyz880rwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1jc3emk</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Chaos Reigns!</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwlnhalgqwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1jc3b2m</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Velvetized Fields of Lavender in nature to help heal the soul 💗</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9qag1nbipwoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1jc32ty</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Nail polish color to match outfit recc</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7r9awh4snwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1jc2qfz</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Looking for a glowy pink with a less intense shimmer load</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jc2qfz/looking_for_a_glowy_pink_with_a_less_intense/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1jc2big</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Bright shimmery greens?</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8ee19wthwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1jc2b8t</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>LA Marathon Calls for a LAM Mani</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc29h6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1jc27jw</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>A perfect soft pink</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc27jw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1jc24rm</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>I need a "refresher" top coat recommendation</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jc24rm/i_need_a_refresher_top_coat_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1jc1xr8</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>My Current St. Patrick's Day Mani</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc1xr8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1jc1usw</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Magnetics Help</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jc1usw/magnetics_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1jc1ljh</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>St. Patty’s rainbow + pot of gold.) Nail art turned out for once!)</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92c8vj52cwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1jc1hr9</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>ILNP Blue Lagoon for my shorties</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2vgt367bwoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1jc13tm</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Someone complimented my nails today 😍</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7c732q48woe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1jc0ptx</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>Alternative to this polish but NOT thermal?</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wiq5jg135woe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1jc05t8</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Nail Polish Color Variation -- is it normal?</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jc05t8/nail_polish_color_variation_is_it_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1jbzz90</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Cuticula recommendations</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czg1aszbzvoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1jbyzqo</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Mooncat - Flight of the monarchs</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyfgoxeorvoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1jbyvlf</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Tell me your favorite brown pinks/dusty roses</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jbyvlf/tell_me_your_favorite_brown_pinksdusty_roses/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1jbym4r</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Jen &amp; Berries and BCB Lacquers</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbym4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1jbxru3</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>My favorite shade of my favorite color 💜</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u201zpnvhvoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1jbwxns</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>My first magnetic!</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mucd6474bvoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1jbwocu</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Queen of Rot 👑🤎</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbwocu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1jbw40f</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>opi infinite shine</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jbw40f/opi_infinite_shine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1jbvxl8</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Dupe for Mooncat Bread and Butterflies</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/907hxy5k2voe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1jbuu03</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>TIFU my Clionadh order</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jbuu03/tifu_my_clionadh_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1jbumu6</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>🍺Guinness Tips🍺</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbumu6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1jbudu8</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>What's your record application time? It's far from perfect, but this is mine - 22 minutes including removal of previous (glitter!) polish</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/07bk9ek3ouoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1jbtvik</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Swatch fridge magnets</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbtvik</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1jbspk8</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>How can I improve the velvet effect?</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/adpzxdjb5uoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1jbsgw3</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>The miracle of oil</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbsgw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1jcecof</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>I tried a new gothic style</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mieh8qpujzoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1jccvct</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>Press-on Set I made for a friend</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jccvct</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1jc9t4v</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Jojo’s bizarre adventure Nails</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc9t4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1jc9cs6</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>Hilma af Klint inspired</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc9cs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1jc6stt</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>Pup approved?</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc6stt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1jc6sfd</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Another nail design</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc6sfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1jc4pn7</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Couple fuzzy kitties 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofqvkw1y0xoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1jc3meo</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Beginner tutorials/info</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jc3meo/beginner_tutorialsinfo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1jc213w</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>cyberpunk</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jc213w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1jc0szg</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>advice on how to do my opposite hand</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jc0szg/advice_on_how_to_do_my_opposite_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1jc0s6a</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>what objects can i use for a dotting tool?</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jc0s6a/what_objects_can_i_use_for_a_dotting_tool/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1jbzlkq</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>Some hand painted work</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jbzlkq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1jbz8ce</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Some work of mine</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5sxxoyktvoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1jbwpzk</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0aswavb9voe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1jbvswx</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Need your help gurlies</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jbvswx/need_your_help_gurlies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1jbuq2o</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>St. Paddy’s Day with a little touch of spring…🍀🌼</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jli59z7eruoe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>